<commit_message>
complete attendance and salary
</commit_message>
<xml_diff>
--- a/MS Excell/Attendance Report+Salary Sheet.xlsx
+++ b/MS Excell/Attendance Report+Salary Sheet.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ATTENDEANCE" sheetId="1" r:id="rId1"/>
+    <sheet name="Salary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="53">
   <si>
     <t>S.NO</t>
   </si>
@@ -127,13 +128,67 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>EMPLOYEE DETAILS</t>
+  </si>
+  <si>
+    <t>WORKING DAYS</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>HRA</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>ALLOWANCES</t>
+  </si>
+  <si>
+    <t>PER DAY INCOME</t>
+  </si>
+  <si>
+    <t>MONTHLY SALARY</t>
+  </si>
+  <si>
+    <t>DEDUCTIONS</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>ESI</t>
+  </si>
+  <si>
+    <t>DEDUCTION</t>
+  </si>
+  <si>
+    <t>EMPLOYEE NET SALARY</t>
+  </si>
+  <si>
+    <t>TOTAL DAYS</t>
+  </si>
+  <si>
+    <t>IN HAND SALARY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +203,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +253,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,10 +342,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -257,8 +358,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,14 +370,67 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -368,6 +525,95 @@
               </a:effectLst>
             </a:rPr>
             <a:t>ATTENDANCE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> DATABASE REPORT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333434</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6210241" cy="533400"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5153084" y="200025"/>
+          <a:ext cx="6210241" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>SALARY</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0" baseline="0">
@@ -671,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,25 +971,25 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -758,7 +1004,7 @@
       <c r="K5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="M5" s="3" t="s">
@@ -779,7 +1025,7 @@
       <c r="R5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -800,7 +1046,7 @@
       <c r="Y5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Z5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="AA5" s="3" t="s">
@@ -821,7 +1067,7 @@
       <c r="AF5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AG5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="AH5" s="3" t="s">
@@ -833,7 +1079,7 @@
       <c r="AJ5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="AL5" s="4" t="s">
@@ -853,13 +1099,13 @@
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="3">
         <v>1</v>
       </c>
@@ -872,7 +1118,7 @@
       <c r="K6" s="3">
         <v>4</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="6">
         <v>5</v>
       </c>
       <c r="M6" s="3">
@@ -893,7 +1139,7 @@
       <c r="R6" s="3">
         <v>11</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="6">
         <v>12</v>
       </c>
       <c r="T6" s="3">
@@ -914,7 +1160,7 @@
       <c r="Y6" s="3">
         <v>18</v>
       </c>
-      <c r="Z6" s="9">
+      <c r="Z6" s="6">
         <v>19</v>
       </c>
       <c r="AA6" s="3">
@@ -935,7 +1181,7 @@
       <c r="AF6" s="3">
         <v>25</v>
       </c>
-      <c r="AG6" s="9">
+      <c r="AG6" s="6">
         <v>26</v>
       </c>
       <c r="AH6" s="3">
@@ -947,7 +1193,7 @@
       <c r="AJ6" s="3">
         <v>29</v>
       </c>
-      <c r="AK6" s="8">
+      <c r="AK6" s="5">
         <v>30</v>
       </c>
       <c r="AL6" s="4" t="s">
@@ -1000,7 +1246,7 @@
       <c r="K7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1021,7 +1267,7 @@
       <c r="R7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="S7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T7" s="2" t="s">
@@ -1042,7 +1288,7 @@
       <c r="Y7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" s="9" t="s">
+      <c r="Z7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AA7" s="2" t="s">
@@ -1063,11 +1309,11 @@
       <c r="AF7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG7" s="9" t="s">
+      <c r="AG7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AI7" s="2" t="s">
         <v>33</v>
@@ -1083,7 +1329,7 @@
       </c>
       <c r="AM7" s="2">
         <f>COUNTIF(H7:AK7,"P")</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AN7" s="2">
         <f>COUNTIF(H7:AK7,"A")</f>
@@ -1091,11 +1337,11 @@
       </c>
       <c r="AO7" s="2">
         <f>COUNTIF(H7:AK7,"L")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AP7" s="2">
         <f>AL7-AN7-AO7</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
@@ -1132,7 +1378,7 @@
       <c r="K8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1153,7 +1399,7 @@
       <c r="R8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="2" t="s">
@@ -1174,7 +1420,7 @@
       <c r="Y8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Z8" s="9" t="s">
+      <c r="Z8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AA8" s="2" t="s">
@@ -1195,7 +1441,7 @@
       <c r="AF8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG8" s="9" t="s">
+      <c r="AG8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AH8" s="2" t="s">
@@ -1264,7 +1510,7 @@
       <c r="K9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -1285,7 +1531,7 @@
       <c r="R9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T9" s="2" t="s">
@@ -1306,7 +1552,7 @@
       <c r="Y9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Z9" s="9" t="s">
+      <c r="Z9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AA9" s="2" t="s">
@@ -1327,7 +1573,7 @@
       <c r="AF9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG9" s="9" t="s">
+      <c r="AG9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AH9" s="2" t="s">
@@ -1396,7 +1642,7 @@
       <c r="K10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -1417,7 +1663,7 @@
       <c r="R10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T10" s="2" t="s">
@@ -1438,7 +1684,7 @@
       <c r="Y10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Z10" s="9" t="s">
+      <c r="Z10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AA10" s="2" t="s">
@@ -1459,7 +1705,7 @@
       <c r="AF10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AG10" s="9" t="s">
+      <c r="AG10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AH10" s="2" t="s">
@@ -1528,7 +1774,7 @@
       <c r="K11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -1549,7 +1795,7 @@
       <c r="R11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T11" s="2" t="s">
@@ -1570,7 +1816,7 @@
       <c r="Y11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Z11" s="9" t="s">
+      <c r="Z11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AA11" s="2" t="s">
@@ -1591,7 +1837,7 @@
       <c r="AF11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AG11" s="9" t="s">
+      <c r="AG11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AH11" s="2" t="s">
@@ -1640,4 +1886,616 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:W22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="13" width="9.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.7109375" customWidth="1"/>
+    <col min="27" max="27" width="4.28515625" customWidth="1"/>
+    <col min="28" max="28" width="4.7109375" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" customWidth="1"/>
+    <col min="30" max="30" width="4.28515625" customWidth="1"/>
+    <col min="31" max="31" width="5.140625" customWidth="1"/>
+    <col min="32" max="32" width="4.5703125" customWidth="1"/>
+    <col min="33" max="33" width="3.7109375" customWidth="1"/>
+    <col min="34" max="34" width="4.28515625" customWidth="1"/>
+    <col min="35" max="35" width="4.7109375" customWidth="1"/>
+    <col min="36" max="36" width="5.5703125" customWidth="1"/>
+    <col min="37" max="37" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="J7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="P7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="T7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+    </row>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+    </row>
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="10">
+        <v>175700010</v>
+      </c>
+      <c r="H11" s="14">
+        <f>ATTENDEANCE!AP7</f>
+        <v>26</v>
+      </c>
+      <c r="J11" s="26">
+        <f>H11*$F$17</f>
+        <v>16900</v>
+      </c>
+      <c r="K11" s="26">
+        <f>J11*$K$18</f>
+        <v>2535</v>
+      </c>
+      <c r="L11" s="26">
+        <f>J11*$K$19</f>
+        <v>3380</v>
+      </c>
+      <c r="M11" s="26">
+        <f>J11*$K$20</f>
+        <v>5070</v>
+      </c>
+      <c r="N11" s="27">
+        <f>J11+K11+L11+M11</f>
+        <v>27885</v>
+      </c>
+      <c r="P11" s="28">
+        <f>J11*$K$21</f>
+        <v>2028</v>
+      </c>
+      <c r="Q11" s="28">
+        <f>J11*$K$22</f>
+        <v>591.5</v>
+      </c>
+      <c r="R11" s="29">
+        <f>P11+Q11</f>
+        <v>2619.5</v>
+      </c>
+      <c r="T11" s="14">
+        <f>ATTENDEANCE!AL7</f>
+        <v>30</v>
+      </c>
+      <c r="U11" s="14">
+        <f>ATTENDEANCE!AP7</f>
+        <v>26</v>
+      </c>
+      <c r="V11" s="26">
+        <f>$F$18</f>
+        <v>19500</v>
+      </c>
+      <c r="W11" s="30">
+        <f>N11-R11</f>
+        <v>25265.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="2">
+        <v>175700011</v>
+      </c>
+      <c r="H12" s="14">
+        <f>ATTENDEANCE!AP8</f>
+        <v>27</v>
+      </c>
+      <c r="J12" s="26">
+        <f t="shared" ref="J12:J15" si="0">H12*$F$17</f>
+        <v>17550</v>
+      </c>
+      <c r="K12" s="26">
+        <f>J12*$K$18</f>
+        <v>2632.5</v>
+      </c>
+      <c r="L12" s="26">
+        <f>J12*$K$19</f>
+        <v>3510</v>
+      </c>
+      <c r="M12" s="26">
+        <f>J12*$K$20</f>
+        <v>5265</v>
+      </c>
+      <c r="N12" s="27">
+        <f t="shared" ref="N12:N15" si="1">J12+K12+L12+M12</f>
+        <v>28957.5</v>
+      </c>
+      <c r="P12" s="28">
+        <f t="shared" ref="P12:P15" si="2">J12*$K$21</f>
+        <v>2106</v>
+      </c>
+      <c r="Q12" s="28">
+        <f t="shared" ref="Q12:Q15" si="3">J12*$K$22</f>
+        <v>614.25000000000011</v>
+      </c>
+      <c r="R12" s="29">
+        <f t="shared" ref="R12:R15" si="4">P12+Q12</f>
+        <v>2720.25</v>
+      </c>
+      <c r="T12" s="14">
+        <f>ATTENDEANCE!AL8</f>
+        <v>30</v>
+      </c>
+      <c r="U12" s="14">
+        <f>ATTENDEANCE!AP8</f>
+        <v>27</v>
+      </c>
+      <c r="V12" s="26">
+        <f t="shared" ref="V12:V15" si="5">$F$18</f>
+        <v>19500</v>
+      </c>
+      <c r="W12" s="30">
+        <f t="shared" ref="W12:W15" si="6">N12-R12</f>
+        <v>26237.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2">
+        <v>175700012</v>
+      </c>
+      <c r="H13" s="14">
+        <f>ATTENDEANCE!AP9</f>
+        <v>29</v>
+      </c>
+      <c r="J13" s="26">
+        <f t="shared" si="0"/>
+        <v>18850</v>
+      </c>
+      <c r="K13" s="26">
+        <f>J13*$K$18</f>
+        <v>2827.5</v>
+      </c>
+      <c r="L13" s="26">
+        <f>J13*$K$19</f>
+        <v>3770</v>
+      </c>
+      <c r="M13" s="26">
+        <f>J13*$K$20</f>
+        <v>5655</v>
+      </c>
+      <c r="N13" s="27">
+        <f t="shared" si="1"/>
+        <v>31102.5</v>
+      </c>
+      <c r="P13" s="28">
+        <f t="shared" si="2"/>
+        <v>2262</v>
+      </c>
+      <c r="Q13" s="28">
+        <f t="shared" si="3"/>
+        <v>659.75000000000011</v>
+      </c>
+      <c r="R13" s="29">
+        <f t="shared" si="4"/>
+        <v>2921.75</v>
+      </c>
+      <c r="T13" s="14">
+        <f>ATTENDEANCE!AL9</f>
+        <v>30</v>
+      </c>
+      <c r="U13" s="14">
+        <f>ATTENDEANCE!AP9</f>
+        <v>29</v>
+      </c>
+      <c r="V13" s="26">
+        <f t="shared" si="5"/>
+        <v>19500</v>
+      </c>
+      <c r="W13" s="30">
+        <f t="shared" si="6"/>
+        <v>28180.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2">
+        <v>175700013</v>
+      </c>
+      <c r="H14" s="14">
+        <f>ATTENDEANCE!AP10</f>
+        <v>27</v>
+      </c>
+      <c r="J14" s="26">
+        <f t="shared" si="0"/>
+        <v>17550</v>
+      </c>
+      <c r="K14" s="26">
+        <f>J14*$K$18</f>
+        <v>2632.5</v>
+      </c>
+      <c r="L14" s="26">
+        <f>J14*$K$19</f>
+        <v>3510</v>
+      </c>
+      <c r="M14" s="26">
+        <f>J14*$K$20</f>
+        <v>5265</v>
+      </c>
+      <c r="N14" s="27">
+        <f t="shared" si="1"/>
+        <v>28957.5</v>
+      </c>
+      <c r="P14" s="28">
+        <f t="shared" si="2"/>
+        <v>2106</v>
+      </c>
+      <c r="Q14" s="28">
+        <f t="shared" si="3"/>
+        <v>614.25000000000011</v>
+      </c>
+      <c r="R14" s="29">
+        <f t="shared" si="4"/>
+        <v>2720.25</v>
+      </c>
+      <c r="T14" s="14">
+        <f>ATTENDEANCE!AL10</f>
+        <v>30</v>
+      </c>
+      <c r="U14" s="14">
+        <f>ATTENDEANCE!AP10</f>
+        <v>27</v>
+      </c>
+      <c r="V14" s="26">
+        <f t="shared" si="5"/>
+        <v>19500</v>
+      </c>
+      <c r="W14" s="30">
+        <f t="shared" si="6"/>
+        <v>26237.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2">
+        <v>175700014</v>
+      </c>
+      <c r="H15" s="14">
+        <f>ATTENDEANCE!AP11</f>
+        <v>26</v>
+      </c>
+      <c r="J15" s="26">
+        <f t="shared" si="0"/>
+        <v>16900</v>
+      </c>
+      <c r="K15" s="26">
+        <f>J15*$K$18</f>
+        <v>2535</v>
+      </c>
+      <c r="L15" s="26">
+        <f>J15*$K$19</f>
+        <v>3380</v>
+      </c>
+      <c r="M15" s="26">
+        <f>J15*$K$20</f>
+        <v>5070</v>
+      </c>
+      <c r="N15" s="27">
+        <f t="shared" si="1"/>
+        <v>27885</v>
+      </c>
+      <c r="P15" s="28">
+        <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="Q15" s="28">
+        <f t="shared" si="3"/>
+        <v>591.5</v>
+      </c>
+      <c r="R15" s="29">
+        <f t="shared" si="4"/>
+        <v>2619.5</v>
+      </c>
+      <c r="T15" s="14">
+        <f>ATTENDEANCE!AL11</f>
+        <v>30</v>
+      </c>
+      <c r="U15" s="14">
+        <f>ATTENDEANCE!AP11</f>
+        <v>26</v>
+      </c>
+      <c r="V15" s="26">
+        <f t="shared" si="5"/>
+        <v>19500</v>
+      </c>
+      <c r="W15" s="30">
+        <f t="shared" si="6"/>
+        <v>25265.5</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="28">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="28">
+        <f>F17*30</f>
+        <v>19500</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="24">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="P7:R8"/>
+    <mergeCell ref="T7:W8"/>
+    <mergeCell ref="A7:H8"/>
+    <mergeCell ref="J7:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>